<commit_message>
test added 22 04 22
</commit_message>
<xml_diff>
--- a/Cases.xlsx
+++ b/Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Study\DiplomMQA\fmh-android\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F0360E-1134-4025-800E-FF754ACF5525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F04F20-45FC-410B-9A85-84BE250B10D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{6B1BD001-B512-4C7A-985E-C3F88C11272E}"/>
+    <workbookView xWindow="51480" yWindow="2295" windowWidth="29040" windowHeight="15720" xr2:uid="{6B1BD001-B512-4C7A-985E-C3F88C11272E}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="181">
   <si>
     <t>№</t>
   </si>
@@ -574,6 +574,9 @@
   </si>
   <si>
     <t>О нас</t>
+  </si>
+  <si>
+    <t>Добавление комментария к жалобе</t>
   </si>
 </sst>
 </file>
@@ -601,7 +604,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -620,6 +623,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -634,7 +643,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -663,6 +672,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Денежный" xfId="1" builtinId="4"/>
@@ -980,14 +993,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4B11D09-2A4D-41FF-B192-494C3CFF5880}">
   <dimension ref="A1:F886"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="56.85546875" customWidth="1"/>
-    <col min="3" max="4" width="33" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" customWidth="1"/>
+    <col min="3" max="3" width="33" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
     <col min="5" max="5" width="70.7109375" customWidth="1"/>
     <col min="6" max="6" width="80.42578125" customWidth="1"/>
   </cols>
@@ -1464,65 +1478,65 @@
       </c>
       <c r="F35" s="6"/>
     </row>
-    <row r="36" spans="1:6" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
+    <row r="36" spans="1:6" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="6">
         <v>14</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E36" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2" t="s">
+    <row r="37" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F37" s="2"/>
-    </row>
-    <row r="38" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2" t="s">
+      <c r="F37" s="6"/>
+    </row>
+    <row r="38" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F38" s="2"/>
-    </row>
-    <row r="39" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2" t="s">
+      <c r="F38" s="6"/>
+    </row>
+    <row r="39" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F39" s="2"/>
-    </row>
-    <row r="40" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2" t="s">
+      <c r="F39" s="6"/>
+    </row>
+    <row r="40" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F40" s="2"/>
+      <c r="F40" s="6"/>
     </row>
     <row r="41" spans="1:6" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
@@ -1584,305 +1598,305 @@
       </c>
       <c r="F45" s="2"/>
     </row>
-    <row r="46" spans="1:6" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
+    <row r="46" spans="1:6" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="6">
         <v>16</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="E46" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="F46" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2" t="s">
+    <row r="47" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F47" s="2"/>
-    </row>
-    <row r="48" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2" t="s">
+      <c r="F47" s="6"/>
+    </row>
+    <row r="48" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F48" s="2"/>
-    </row>
-    <row r="49" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2" t="s">
+      <c r="F48" s="6"/>
+    </row>
+    <row r="49" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F49" s="2"/>
-    </row>
-    <row r="50" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2" t="s">
+      <c r="F49" s="6"/>
+    </row>
+    <row r="50" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="6"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F50" s="2"/>
-    </row>
-    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
+      <c r="F50" s="6"/>
+    </row>
+    <row r="51" spans="1:6" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="6">
         <v>17</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D51" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E51" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="F51" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1" t="s">
+    <row r="52" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="6"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F52" s="1"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1" t="s">
+      <c r="F52" s="6"/>
+    </row>
+    <row r="53" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="6"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F53" s="1"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1" t="s">
+      <c r="F53" s="6"/>
+    </row>
+    <row r="54" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="6"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F54" s="1"/>
-    </row>
-    <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
+      <c r="F54" s="6"/>
+    </row>
+    <row r="55" spans="1:6" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="6">
         <v>18</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D55" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="E55" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="F55" s="6" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1" t="s">
+    <row r="56" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="6"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F56" s="1"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1" t="s">
+      <c r="F56" s="6"/>
+    </row>
+    <row r="57" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="6"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F57" s="1"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1" t="s">
+      <c r="F57" s="6"/>
+    </row>
+    <row r="58" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="6"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F58" s="1"/>
-    </row>
-    <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
+      <c r="F58" s="6"/>
+    </row>
+    <row r="59" spans="1:6" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="12">
         <v>19</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="D59" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E59" s="1" t="s">
+      <c r="D59" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="E59" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F59" s="1" t="s">
+      <c r="F59" s="12" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1" t="s">
+    <row r="60" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="12"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="F60" s="1"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1" t="s">
+      <c r="F60" s="12"/>
+    </row>
+    <row r="61" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="12"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F61" s="1"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1" t="s">
+      <c r="F61" s="12"/>
+    </row>
+    <row r="62" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="12"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="F62" s="1"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1" t="s">
+      <c r="F62" s="12"/>
+    </row>
+    <row r="63" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="12"/>
+      <c r="B63" s="12"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="F63" s="1"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1" t="s">
+      <c r="F63" s="12"/>
+    </row>
+    <row r="64" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="12"/>
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F64" s="1"/>
-    </row>
-    <row r="65" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
+      <c r="F64" s="12"/>
+    </row>
+    <row r="65" spans="1:6" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A65" s="6">
         <v>20</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D65" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="E65" s="1" t="s">
+      <c r="E65" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F65" s="1" t="s">
+      <c r="F65" s="6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1" t="s">
+    <row r="66" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="6"/>
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F66" s="1"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1" t="s">
+      <c r="F66" s="6"/>
+    </row>
+    <row r="67" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="6"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F67" s="1"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1" t="s">
+      <c r="F67" s="6"/>
+    </row>
+    <row r="68" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="6"/>
+      <c r="B68" s="6"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="F68" s="1"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1" t="s">
+      <c r="F68" s="6"/>
+    </row>
+    <row r="69" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="6"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="F69" s="1"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1" t="s">
+      <c r="F69" s="6"/>
+    </row>
+    <row r="70" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="6"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="F70" s="1"/>
+      <c r="F70" s="6"/>
     </row>
     <row r="71" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="1">

</xml_diff>

<commit_message>
some tests added 28 04 22
</commit_message>
<xml_diff>
--- a/Cases.xlsx
+++ b/Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Study\DiplomMQA\fmh-android\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F04F20-45FC-410B-9A85-84BE250B10D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA6B4EE-8F7B-459A-B4DA-DEB7627F9514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51480" yWindow="2295" windowWidth="29040" windowHeight="15720" xr2:uid="{6B1BD001-B512-4C7A-985E-C3F88C11272E}"/>
   </bookViews>
@@ -993,8 +993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4B11D09-2A4D-41FF-B192-494C3CFF5880}">
   <dimension ref="A1:F886"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,7 +1006,7 @@
     <col min="6" max="6" width="80.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1070,7 +1070,7 @@
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -1108,7 +1108,7 @@
       </c>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>4</v>
       </c>
@@ -1146,7 +1146,7 @@
       </c>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>5</v>
       </c>
@@ -1658,7 +1658,7 @@
       </c>
       <c r="F50" s="6"/>
     </row>
-    <row r="51" spans="1:6" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
         <v>17</v>
       </c>
@@ -1828,75 +1828,75 @@
       </c>
       <c r="F64" s="12"/>
     </row>
-    <row r="65" spans="1:6" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="6">
+    <row r="65" spans="1:6" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A65" s="12">
         <v>20</v>
       </c>
-      <c r="B65" s="6" t="s">
+      <c r="B65" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C65" s="6" t="s">
+      <c r="C65" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="D65" s="6" t="s">
+      <c r="D65" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="E65" s="6" t="s">
+      <c r="E65" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F65" s="6" t="s">
+      <c r="F65" s="12" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="66" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="6"/>
-      <c r="B66" s="6"/>
-      <c r="C66" s="6"/>
-      <c r="D66" s="6"/>
-      <c r="E66" s="6" t="s">
+    <row r="66" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="12"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="F66" s="6"/>
-    </row>
-    <row r="67" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="6"/>
-      <c r="B67" s="6"/>
-      <c r="C67" s="6"/>
-      <c r="D67" s="6"/>
-      <c r="E67" s="6" t="s">
+      <c r="F66" s="12"/>
+    </row>
+    <row r="67" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="12"/>
+      <c r="B67" s="12"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F67" s="6"/>
-    </row>
-    <row r="68" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="6"/>
-      <c r="B68" s="6"/>
-      <c r="C68" s="6"/>
-      <c r="D68" s="6"/>
-      <c r="E68" s="6" t="s">
+      <c r="F67" s="12"/>
+    </row>
+    <row r="68" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="12"/>
+      <c r="B68" s="12"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="F68" s="6"/>
-    </row>
-    <row r="69" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="6"/>
-      <c r="B69" s="6"/>
-      <c r="C69" s="6"/>
-      <c r="D69" s="6"/>
-      <c r="E69" s="6" t="s">
+      <c r="F68" s="12"/>
+    </row>
+    <row r="69" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="12"/>
+      <c r="B69" s="12"/>
+      <c r="C69" s="12"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="F69" s="6"/>
-    </row>
-    <row r="70" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="6"/>
-      <c r="B70" s="6"/>
-      <c r="C70" s="6"/>
-      <c r="D70" s="6"/>
-      <c r="E70" s="6" t="s">
+      <c r="F69" s="12"/>
+    </row>
+    <row r="70" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="12"/>
+      <c r="B70" s="12"/>
+      <c r="C70" s="12"/>
+      <c r="D70" s="12"/>
+      <c r="E70" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="F70" s="6"/>
+      <c r="F70" s="12"/>
     </row>
     <row r="71" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
@@ -2598,7 +2598,7 @@
       </c>
       <c r="F133" s="1"/>
     </row>
-    <row r="134" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>28</v>
       </c>
@@ -3608,7 +3608,7 @@
       </c>
       <c r="F219" s="1"/>
     </row>
-    <row r="220" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>43</v>
       </c>
@@ -3678,7 +3678,7 @@
       </c>
       <c r="F225" s="1"/>
     </row>
-    <row r="226" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>44</v>
       </c>
@@ -3828,7 +3828,7 @@
       </c>
       <c r="F238" s="1"/>
     </row>
-    <row r="239" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>46</v>
       </c>
@@ -3908,7 +3908,7 @@
       </c>
       <c r="F245" s="1"/>
     </row>
-    <row r="246" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
01 06 22 tests added
</commit_message>
<xml_diff>
--- a/Cases.xlsx
+++ b/Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Study\DiplomMQA\fmh-android\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45853345-38D6-417F-B9C0-DFE77F306336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA86DE3D-E9DD-4A01-8F58-085396E0FC6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="2295" windowWidth="29040" windowHeight="15720" xr2:uid="{6B1BD001-B512-4C7A-985E-C3F88C11272E}"/>
+    <workbookView xWindow="51390" yWindow="3000" windowWidth="29010" windowHeight="15345" xr2:uid="{6B1BD001-B512-4C7A-985E-C3F88C11272E}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="184">
   <si>
     <t>№</t>
   </si>
@@ -577,6 +577,15 @@
   </si>
   <si>
     <t>Добавление комментария к жалобе</t>
+  </si>
+  <si>
+    <t>Создается а не должно</t>
+  </si>
+  <si>
+    <t>Обрезает до 50 символов и создает</t>
+  </si>
+  <si>
+    <t>Возможен ввод более 255 символов</t>
   </si>
 </sst>
 </file>
@@ -675,9 +684,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -696,6 +702,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Денежный" xfId="1" builtinId="4"/>
@@ -1013,8 +1022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4B11D09-2A4D-41FF-B192-494C3CFF5880}">
   <dimension ref="A1:F255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,877 +1055,883 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
+    <row r="2" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
+    <row r="3" spans="1:6" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11" t="s">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11" t="s">
+    <row r="4" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="11"/>
-    </row>
-    <row r="5" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" spans="1:6" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11" t="s">
+    <row r="6" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="11"/>
-    </row>
-    <row r="7" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11" t="s">
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="11"/>
-    </row>
-    <row r="8" spans="1:6" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
+      <c r="F7" s="10"/>
+    </row>
+    <row r="8" spans="1:6" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
         <v>4</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13" t="s">
+      <c r="C8" s="12"/>
+      <c r="D8" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13" t="s">
+    <row r="9" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="13"/>
-    </row>
-    <row r="10" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13" t="s">
+      <c r="F9" s="12"/>
+    </row>
+    <row r="10" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="13"/>
-    </row>
-    <row r="11" spans="1:6" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="13">
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="1:6" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
         <v>5</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="D11" s="13" t="s">
+      <c r="C11" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="E11" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="13" t="s">
+      <c r="E11" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="13"/>
-    </row>
-    <row r="13" spans="1:6" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
+    <row r="12" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="1:6" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
         <v>6</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="D13" s="13" t="s">
+      <c r="C13" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
+    <row r="14" spans="1:6" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
         <v>7</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="D14" s="13" t="s">
+      <c r="C14" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="D14" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13" t="s">
+    <row r="15" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="13"/>
-    </row>
-    <row r="16" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="13"/>
-    </row>
-    <row r="17" spans="1:6" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="13">
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:6" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
         <v>8</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="D17" s="13" t="s">
+      <c r="C17" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="E17" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="13" t="s">
+      <c r="E17" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13" t="s">
+    <row r="18" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="13"/>
-    </row>
-    <row r="19" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="13"/>
-    </row>
-    <row r="20" spans="1:6" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="13">
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="1:6" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
         <v>9</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="D20" s="13" t="s">
+      <c r="C20" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="D20" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="E20" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="13" t="s">
+      <c r="E20" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13" t="s">
+    <row r="21" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F21" s="13"/>
-    </row>
-    <row r="22" spans="1:6" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="13">
+      <c r="F21" s="12"/>
+    </row>
+    <row r="22" spans="1:6" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="12">
         <v>10</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="D22" s="13" t="s">
+      <c r="C22" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="E22" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="13" t="s">
+      <c r="E22" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13" t="s">
+    <row r="23" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F23" s="13" t="s">
+      <c r="F23" s="12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="13">
+    <row r="24" spans="1:6" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="12">
         <v>11</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="D24" s="13" t="s">
+      <c r="C24" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="D24" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E24" s="12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25" s="13"/>
-    </row>
-    <row r="26" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13" t="s">
+    <row r="25" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="12"/>
+    </row>
+    <row r="26" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F26" s="13"/>
-    </row>
-    <row r="27" spans="1:6" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="16">
+      <c r="F26" s="12"/>
+    </row>
+    <row r="27" spans="1:6" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="15">
         <v>12</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="D27" s="16" t="s">
+      <c r="C27" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="D27" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="E27" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27" s="16" t="s">
+      <c r="E27" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16" t="s">
+    <row r="28" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F28" s="16"/>
-    </row>
-    <row r="29" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16" t="s">
+      <c r="F28" s="15"/>
+    </row>
+    <row r="29" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="F29" s="16"/>
-    </row>
-    <row r="30" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16" t="s">
+      <c r="F29" s="15"/>
+    </row>
+    <row r="30" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F30" s="16"/>
-    </row>
-    <row r="31" spans="1:6" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="16">
+      <c r="F30" s="15"/>
+    </row>
+    <row r="31" spans="1:6" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="15">
         <v>13</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="D31" s="16" t="s">
+      <c r="C31" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="D31" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="E31" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F31" s="16" t="s">
+      <c r="E31" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16" t="s">
+    <row r="32" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F32" s="16"/>
-    </row>
-    <row r="33" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16" t="s">
+      <c r="F32" s="15"/>
+    </row>
+    <row r="33" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F33" s="16"/>
-    </row>
-    <row r="34" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16" t="s">
+      <c r="F33" s="15"/>
+    </row>
+    <row r="34" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="F34" s="16"/>
-    </row>
-    <row r="35" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16" t="s">
+      <c r="F34" s="15"/>
+    </row>
+    <row r="35" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="15"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F35" s="16"/>
-    </row>
-    <row r="36" spans="1:6" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="6">
-        <v>14</v>
-      </c>
-      <c r="B36" s="6" t="s">
+      <c r="F35" s="15"/>
+    </row>
+    <row r="36" spans="1:6" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="15">
+        <v>14</v>
+      </c>
+      <c r="B36" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C36" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="D36" s="6" t="s">
+      <c r="C36" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="D36" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="E36" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F36" s="6" t="s">
+      <c r="E36" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" s="15" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6" t="s">
+    <row r="37" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="15"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F37" s="6"/>
-    </row>
-    <row r="38" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6" t="s">
+      <c r="F37" s="15"/>
+    </row>
+    <row r="38" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="15"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F38" s="6"/>
-    </row>
-    <row r="39" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6" t="s">
+      <c r="F38" s="15"/>
+    </row>
+    <row r="39" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="15"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="F39" s="6"/>
-    </row>
-    <row r="40" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6" t="s">
+      <c r="F39" s="15"/>
+    </row>
+    <row r="40" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="15"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F40" s="6"/>
-    </row>
-    <row r="41" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
+      <c r="F40" s="15"/>
+    </row>
+    <row r="41" spans="1:6" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="6">
         <v>15</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D41" s="2" t="s">
+      <c r="C41" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="E41" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F41" s="2" t="s">
+      <c r="E41" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F41" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2" t="s">
+    <row r="42" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F42" s="9"/>
-    </row>
-    <row r="43" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2" t="s">
+      <c r="F42" s="17"/>
+    </row>
+    <row r="43" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F43" s="2"/>
-    </row>
-    <row r="44" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2" t="s">
+      <c r="F43" s="6"/>
+    </row>
+    <row r="44" spans="1:6" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="F44" s="2"/>
-    </row>
-    <row r="45" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2" t="s">
+      <c r="F44" s="6"/>
+    </row>
+    <row r="45" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F45" s="2"/>
-    </row>
-    <row r="46" spans="1:6" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="6">
+      <c r="F45" s="6"/>
+    </row>
+    <row r="46" spans="1:6" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="15">
         <v>16</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="D46" s="6" t="s">
+      <c r="C46" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="D46" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="E46" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F46" s="6" t="s">
+      <c r="E46" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F46" s="15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6" t="s">
+    <row r="47" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="15"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F47" s="6"/>
-    </row>
-    <row r="48" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6" t="s">
+      <c r="F47" s="15"/>
+    </row>
+    <row r="48" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="15"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F48" s="6"/>
-    </row>
-    <row r="49" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6" t="s">
+      <c r="F48" s="15"/>
+    </row>
+    <row r="49" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="15"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="F49" s="6"/>
-    </row>
-    <row r="50" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6" t="s">
+      <c r="F49" s="15"/>
+    </row>
+    <row r="50" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="15"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F50" s="6"/>
-    </row>
-    <row r="51" spans="1:6" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51" s="6">
+      <c r="F50" s="15"/>
+    </row>
+    <row r="51" spans="1:6" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="15">
         <v>17</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B51" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C51" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="D51" s="6" t="s">
+      <c r="C51" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="D51" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="E51" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F51" s="6" t="s">
+      <c r="E51" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F51" s="15" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="6"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6" t="s">
+    <row r="52" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="15"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F52" s="6"/>
-    </row>
-    <row r="53" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="6"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6" t="s">
+      <c r="F52" s="15"/>
+    </row>
+    <row r="53" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="15"/>
+      <c r="B53" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F53" s="6"/>
-    </row>
-    <row r="54" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="6"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6" t="s">
+      <c r="F53" s="15"/>
+    </row>
+    <row r="54" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="15"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="F54" s="6"/>
-    </row>
-    <row r="55" spans="1:6" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="6">
+      <c r="F54" s="15"/>
+    </row>
+    <row r="55" spans="1:6" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="15">
         <v>18</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B55" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C55" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="D55" s="6" t="s">
+      <c r="C55" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="D55" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="E55" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F55" s="6" t="s">
+      <c r="E55" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F55" s="15" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="56" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="6"/>
-      <c r="B56" s="6"/>
-      <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6" t="s">
+    <row r="56" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="15"/>
+      <c r="B56" s="15"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F56" s="6"/>
-    </row>
-    <row r="57" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="6"/>
-      <c r="B57" s="6"/>
-      <c r="C57" s="6"/>
-      <c r="D57" s="6"/>
-      <c r="E57" s="6" t="s">
+      <c r="F56" s="15"/>
+    </row>
+    <row r="57" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="15"/>
+      <c r="B57" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F57" s="6"/>
-    </row>
-    <row r="58" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="6"/>
-      <c r="B58" s="6"/>
-      <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6" t="s">
+      <c r="F57" s="15"/>
+    </row>
+    <row r="58" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="15"/>
+      <c r="B58" s="15"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="F58" s="6"/>
-    </row>
-    <row r="59" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A59" s="11">
+      <c r="F58" s="15"/>
+    </row>
+    <row r="59" spans="1:6" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
         <v>19</v>
       </c>
-      <c r="B59" s="11" t="s">
+      <c r="B59" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C59" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="D59" s="11" t="s">
+      <c r="C59" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E59" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F59" s="11" t="s">
+      <c r="E59" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F59" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="60" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="11"/>
-      <c r="B60" s="11"/>
-      <c r="C60" s="11"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="11" t="s">
+    <row r="60" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F60" s="11"/>
-    </row>
-    <row r="61" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="11"/>
-      <c r="B61" s="11"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11" t="s">
+      <c r="F60" s="2"/>
+    </row>
+    <row r="61" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F61" s="11"/>
-    </row>
-    <row r="62" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="11"/>
-      <c r="B62" s="11"/>
-      <c r="C62" s="11"/>
-      <c r="D62" s="11"/>
-      <c r="E62" s="11" t="s">
+      <c r="F61" s="2"/>
+    </row>
+    <row r="62" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F62" s="11"/>
-    </row>
-    <row r="63" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="11"/>
-      <c r="B63" s="11"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="11"/>
-      <c r="E63" s="11" t="s">
+      <c r="F62" s="2"/>
+    </row>
+    <row r="63" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="2"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F63" s="11"/>
-    </row>
-    <row r="64" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="11"/>
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
-      <c r="E64" s="11" t="s">
+      <c r="F63" s="2"/>
+    </row>
+    <row r="64" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="2"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F64" s="11"/>
-    </row>
-    <row r="65" spans="1:6" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="11">
+      <c r="F64" s="2"/>
+    </row>
+    <row r="65" spans="1:6" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
         <v>20</v>
       </c>
-      <c r="B65" s="11" t="s">
+      <c r="B65" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C65" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="D65" s="11" t="s">
+      <c r="C65" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D65" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="E65" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F65" s="11" t="s">
+      <c r="E65" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F65" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="66" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="11"/>
-      <c r="B66" s="11"/>
-      <c r="C66" s="11"/>
-      <c r="D66" s="11"/>
-      <c r="E66" s="11" t="s">
+    <row r="66" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F66" s="11"/>
-    </row>
-    <row r="67" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="11"/>
-      <c r="B67" s="11"/>
-      <c r="C67" s="11"/>
-      <c r="D67" s="11"/>
-      <c r="E67" s="11" t="s">
+      <c r="F66" s="2"/>
+    </row>
+    <row r="67" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F67" s="11"/>
-    </row>
-    <row r="68" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="11"/>
-      <c r="B68" s="11"/>
-      <c r="C68" s="11"/>
-      <c r="D68" s="11"/>
-      <c r="E68" s="11" t="s">
+      <c r="F67" s="2"/>
+    </row>
+    <row r="68" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F68" s="11"/>
-    </row>
-    <row r="69" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="11"/>
-      <c r="B69" s="11"/>
-      <c r="C69" s="11"/>
-      <c r="D69" s="11"/>
-      <c r="E69" s="11" t="s">
+      <c r="F68" s="2"/>
+    </row>
+    <row r="69" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F69" s="11"/>
-    </row>
-    <row r="70" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="11"/>
-      <c r="B70" s="11"/>
-      <c r="C70" s="11"/>
-      <c r="D70" s="11"/>
-      <c r="E70" s="11" t="s">
+      <c r="F69" s="2"/>
+    </row>
+    <row r="70" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="2"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F70" s="11"/>
+      <c r="F70" s="2"/>
     </row>
     <row r="71" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
@@ -2908,7 +2923,7 @@
       <c r="C158" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D158" s="10" t="s">
+      <c r="D158" s="9" t="s">
         <v>175</v>
       </c>
       <c r="E158" s="1" t="s">

</xml_diff>

<commit_message>
object's and steps updated
</commit_message>
<xml_diff>
--- a/Cases.xlsx
+++ b/Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Study\DiplomMQA\fmh-android\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B2D18C-3428-4D2E-98E2-AA70F4492375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8433E76-A717-44BC-B3A5-0717A8A9D300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51480" yWindow="2295" windowWidth="29040" windowHeight="15720" xr2:uid="{6B1BD001-B512-4C7A-985E-C3F88C11272E}"/>
   </bookViews>
@@ -664,7 +664,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₽&quot;_-;\-* #,##0.00\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -676,6 +676,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -721,7 +728,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -763,6 +770,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Денежный" xfId="1" builtinId="4"/>
@@ -1080,8 +1094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4B11D09-2A4D-41FF-B192-494C3CFF5880}">
   <dimension ref="A1:H254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A235" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H153" sqref="H153"/>
+    <sheetView tabSelected="1" topLeftCell="A166" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D244" sqref="D244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4640,99 +4654,99 @@
       <c r="G245" s="12"/>
       <c r="H245" s="12"/>
     </row>
-    <row r="246" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A246" s="1">
+    <row r="246" spans="1:8" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A246" s="17">
         <v>47</v>
       </c>
-      <c r="B246" s="1" t="s">
+      <c r="B246" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="C246" s="1" t="s">
+      <c r="C246" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="D246" s="1" t="s">
+      <c r="D246" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="E246" s="1" t="s">
+      <c r="E246" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F246" s="1" t="s">
+      <c r="F246" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="G246" s="14"/>
-      <c r="H246" s="14"/>
-    </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A247" s="1"/>
-      <c r="B247" s="1"/>
-      <c r="C247" s="1"/>
-      <c r="D247" s="1"/>
-      <c r="E247" s="1" t="s">
+      <c r="G246" s="18"/>
+      <c r="H246" s="18"/>
+    </row>
+    <row r="247" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A247" s="17"/>
+      <c r="B247" s="17"/>
+      <c r="C247" s="17"/>
+      <c r="D247" s="17"/>
+      <c r="E247" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F247" s="1"/>
-      <c r="G247" s="14"/>
-      <c r="H247" s="14"/>
-    </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A248" s="1"/>
-      <c r="B248" s="1"/>
-      <c r="C248" s="1"/>
-      <c r="D248" s="1"/>
-      <c r="E248" s="1" t="s">
+      <c r="F247" s="17"/>
+      <c r="G247" s="18"/>
+      <c r="H247" s="18"/>
+    </row>
+    <row r="248" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A248" s="17"/>
+      <c r="B248" s="17"/>
+      <c r="C248" s="17"/>
+      <c r="D248" s="17"/>
+      <c r="E248" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="F248" s="1"/>
-      <c r="G248" s="14"/>
-      <c r="H248" s="14"/>
-    </row>
-    <row r="249" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A249" s="1"/>
-      <c r="B249" s="1"/>
-      <c r="C249" s="1"/>
-      <c r="D249" s="1"/>
-      <c r="E249" s="1" t="s">
+      <c r="F248" s="17"/>
+      <c r="G248" s="18"/>
+      <c r="H248" s="18"/>
+    </row>
+    <row r="249" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A249" s="17"/>
+      <c r="B249" s="17"/>
+      <c r="C249" s="17"/>
+      <c r="D249" s="17"/>
+      <c r="E249" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="F249" s="1"/>
-      <c r="G249" s="14"/>
-      <c r="H249" s="14"/>
-    </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A250" s="1"/>
-      <c r="B250" s="1"/>
-      <c r="C250" s="1"/>
-      <c r="D250" s="1"/>
-      <c r="E250" s="1" t="s">
+      <c r="F249" s="17"/>
+      <c r="G249" s="18"/>
+      <c r="H249" s="18"/>
+    </row>
+    <row r="250" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A250" s="17"/>
+      <c r="B250" s="17"/>
+      <c r="C250" s="17"/>
+      <c r="D250" s="17"/>
+      <c r="E250" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="F250" s="1"/>
-      <c r="G250" s="14"/>
-      <c r="H250" s="14"/>
-    </row>
-    <row r="251" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A251" s="1"/>
-      <c r="B251" s="1"/>
-      <c r="C251" s="1"/>
-      <c r="D251" s="1"/>
-      <c r="E251" s="1" t="s">
+      <c r="F250" s="17"/>
+      <c r="G250" s="18"/>
+      <c r="H250" s="18"/>
+    </row>
+    <row r="251" spans="1:8" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A251" s="17"/>
+      <c r="B251" s="17"/>
+      <c r="C251" s="17"/>
+      <c r="D251" s="17"/>
+      <c r="E251" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="F251" s="1"/>
-      <c r="G251" s="14"/>
-      <c r="H251" s="14"/>
-    </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A252" s="1"/>
-      <c r="B252" s="1"/>
-      <c r="C252" s="1"/>
-      <c r="D252" s="1"/>
-      <c r="E252" s="1" t="s">
+      <c r="F251" s="17"/>
+      <c r="G251" s="18"/>
+      <c r="H251" s="18"/>
+    </row>
+    <row r="252" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A252" s="17"/>
+      <c r="B252" s="17"/>
+      <c r="C252" s="17"/>
+      <c r="D252" s="17"/>
+      <c r="E252" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="F252" s="1"/>
-      <c r="G252" s="14"/>
-      <c r="H252" s="14"/>
+      <c r="F252" s="17"/>
+      <c r="G252" s="18"/>
+      <c r="H252" s="18"/>
     </row>
     <row r="253" spans="1:8" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A253" s="8">

</xml_diff>